<commit_message>
emergencyExit fix: caller check
</commit_message>
<xml_diff>
--- a/gas.xlsx
+++ b/gas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjp\Desktop\MocaGithub\13. StakingPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE903FE-ADCE-4429-A217-1C704B478668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DAA660-A2C3-4855-8A46-2FE9AFF86F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47850" yWindow="5070" windowWidth="28800" windowHeight="15345" xr2:uid="{E4A2D2C6-D319-4EB2-99BD-DADC575900BD}"/>
+    <workbookView xWindow="6510" yWindow="4305" windowWidth="28800" windowHeight="15345" xr2:uid="{E4A2D2C6-D319-4EB2-99BD-DADC575900BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>User Fn</t>
   </si>
@@ -66,12 +66,6 @@
     <t>comment</t>
   </si>
   <si>
-    <t>gas cost after 2 distributions have been set up</t>
-  </si>
-  <si>
-    <t>hash</t>
-  </si>
-  <si>
     <t>0xe545d7caec13edcc86c79bf55978ddfa6717e026bfb7cd01894f9ab492aa62be</t>
   </si>
   <si>
@@ -121,13 +115,73 @@
   </si>
   <si>
     <t>1,196,346 </t>
+  </si>
+  <si>
+    <t>0x773f5a7375b1e00c9dcbc60f3c5122ada176c7f63c566aab562bd2c99c49516d</t>
+  </si>
+  <si>
+    <t>1,296,466 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>stakeTokens_hash</t>
+  </si>
+  <si>
+    <t>0xed58045803e69231b066edfa13d42c4c8aa94b3e2a15d862a108f1f429c8cb76</t>
+  </si>
+  <si>
+    <t>StakingPro</t>
+  </si>
+  <si>
+    <t>StakingPro | Address 0x14f2a22c97ae2890e73cb15b1c0e42a8a0821223 | BaseScan</t>
+  </si>
+  <si>
+    <t>0xc97b7a5947ef33b5cc58860359eda7c56ebccd50d078ba56ca7b4ba04d05c88a</t>
+  </si>
+  <si>
+    <t>gas costs for updating 1 distribution, id:0 is returned early within _calculateDistributionIndex</t>
+  </si>
+  <si>
+    <t>however, the loops of userAccounts and vaultAccounts are still accounted</t>
+  </si>
+  <si>
+    <t>0xb7f5dcdbe13d96964a25df65cfddc7285b419fea3870a7c25cee8ec89f775d83</t>
+  </si>
+  <si>
+    <t>1,597,011 </t>
+  </si>
+  <si>
+    <t>0x087ad48bdd51e74d18ede4b539137a9953f7f5f9081ba03e153a61f70dd3bbe0</t>
+  </si>
+  <si>
+    <t>0x2497d8e8522add92e674aebf45e3dde040a8d3a3bf6736e2c18c61ca24b730d7</t>
+  </si>
+  <si>
+    <t>0x1862e87ddcbdd8e473796872b9510b95f5e31c7dff0422d8388d7ccfc10d12be</t>
+  </si>
+  <si>
+    <t>https://base.blockscout.com/blocks</t>
+  </si>
+  <si>
+    <t>Gas used</t>
+  </si>
+  <si>
+    <t>Gas limit</t>
+  </si>
+  <si>
+    <t>(fixed for all blocks)</t>
+  </si>
+  <si>
+    <t>(rough average)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,8 +224,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,8 +281,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -205,41 +308,158 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -266,9 +486,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>326737</xdr:colOff>
+      <xdr:colOff>241012</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>152980</xdr:rowOff>
+      <xdr:rowOff>144697</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -312,7 +532,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>467228</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>63126</xdr:rowOff>
+      <xdr:rowOff>54843</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -645,266 +865,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF862AD1-CC88-47F3-80C2-E6377CA3DCC0}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="H1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="17">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="12" t="s">
-        <v>24</v>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19" t="s">
+        <v>22</v>
       </c>
       <c r="M2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="20">
         <v>1</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="22">
         <v>389670</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>10</v>
+      <c r="E3" s="23" t="s">
+        <v>35</v>
       </c>
       <c r="M3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="20">
         <v>2</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="22">
         <v>702381</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3">
+      <c r="E4" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="20">
         <f>B4+1</f>
         <v>3</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="22">
         <v>674437</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="26" t="s">
+        <v>29</v>
+      </c>
       <c r="M5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="20">
         <f t="shared" ref="B6:B16" si="0">B5+1</f>
         <v>4</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="22">
         <v>783324</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3">
+      <c r="E6" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="20">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="3"/>
+      <c r="C7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>29</v>
+      </c>
       <c r="M7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="3"/>
+      <c r="C8" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>29</v>
+      </c>
       <c r="M8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="20">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="22">
         <v>996200</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3">
+      <c r="E9" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="22">
         <v>1096257</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3">
+      <c r="E10" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="20">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="J11" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3">
+      <c r="C11" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="27">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3">
+      <c r="C12" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="20">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3">
+      <c r="C13" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="22">
+        <v>1396616</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="20">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3">
+      <c r="C14" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="22">
+        <v>1496798</v>
+      </c>
+      <c r="E14" s="26"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="20">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3">
+      <c r="C15" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="20">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J31" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J32" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
+      <c r="C16" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="22">
+        <v>1511511</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="20">
+        <v>15</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="22">
+        <v>1697254</v>
+      </c>
+      <c r="E17" s="26"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31">
+        <v>16</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="33">
+        <v>2393523</v>
+      </c>
+      <c r="E18" s="34"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C19"/>
+      <c r="D19"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C20"/>
+      <c r="D20"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="8">
+        <v>264000000</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="8">
+        <v>40000000</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J31" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I1" r:id="rId1" display="https://sepolia.basescan.org/address/0x14f2a22c97ae2890e73cb15b1c0e42a8a0821223" xr:uid="{7E49AA2A-CC8D-495D-9384-4372F05ACC37}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>